<commit_message>
Add structure and conformations to .docx\review
</commit_message>
<xml_diff>
--- a/references.xlsx
+++ b/references.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yaz008\Desktop\literature-review\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83A7400D-A6C7-4016-BF5F-4CB408856554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{866EB387-00CC-4021-93F9-4DA6BD8D6E3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="22272" windowHeight="14616" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Fact</t>
   </si>
@@ -37,13 +37,22 @@
   </si>
   <si>
     <t>Reference</t>
+  </si>
+  <si>
+    <t>15 kDa subunit epsilon</t>
+  </si>
+  <si>
+    <t>15 kDa</t>
+  </si>
+  <si>
+    <t>file:///C:/Users/yaz008/Desktop/ATP-syntase/literature/Feniouk_BJ_10_epsilon_transitions.pdf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -68,6 +77,14 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -141,15 +158,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -164,8 +182,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -444,17 +466,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="103" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="6.77734375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.77734375" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -472,8 +493,22 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{2CF254D5-05A5-471E-AC86-EF32378CF0B2}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>